<commit_message>
Me agregué más tareas.
</commit_message>
<xml_diff>
--- a/Tareas.xlsx
+++ b/Tareas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="70">
   <si>
     <t xml:space="preserve">Sección</t>
   </si>
@@ -368,7 +368,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -410,6 +410,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -496,21 +500,19 @@
   </sheetPr>
   <dimension ref="A2:K34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.015306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.3214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.4540816326531"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.5408163265306"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.68367346938776"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.015306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.8775510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.0969387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.6173469387755"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -625,6 +627,9 @@
       <c r="D8" s="9" t="s">
         <v>19</v>
       </c>
+      <c r="E8" s="0" t="s">
+        <v>15</v>
+      </c>
       <c r="F8" s="6"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -636,6 +641,9 @@
       <c r="C9" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="E9" s="0" t="s">
+        <v>15</v>
+      </c>
       <c r="F9" s="6"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -649,6 +657,9 @@
       <c r="C10" s="9" t="s">
         <v>22</v>
       </c>
+      <c r="E10" s="0" t="s">
+        <v>15</v>
+      </c>
       <c r="F10" s="6"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -660,6 +671,9 @@
       <c r="C11" s="9" t="s">
         <v>23</v>
       </c>
+      <c r="E11" s="0" t="s">
+        <v>15</v>
+      </c>
       <c r="F11" s="6"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -671,6 +685,9 @@
       <c r="C12" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="E12" s="0" t="s">
+        <v>15</v>
+      </c>
       <c r="F12" s="6"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -693,16 +710,17 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="22.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="11" t="s">
         <v>29</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>30</v>
       </c>
+      <c r="E14" s="4"/>
       <c r="F14" s="6"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
@@ -751,7 +769,7 @@
       <c r="K17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="0" t="s">

</xml_diff>